<commit_message>
fetch and blog and blog category
</commit_message>
<xml_diff>
--- a/edus project timeline and cost 21-april-2025.xlsx
+++ b/edus project timeline and cost 21-april-2025.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="132">
   <si>
     <t>admin_permissions</t>
   </si>
@@ -409,6 +409,24 @@
   </si>
   <si>
     <t>fetch user purchase chapter - pdf -video url -summary-etc</t>
+  </si>
+  <si>
+    <t>create blog category</t>
+  </si>
+  <si>
+    <t>create blog</t>
+  </si>
+  <si>
+    <t>Get blog detail  by blog_id</t>
+  </si>
+  <si>
+    <t>pending</t>
+  </si>
+  <si>
+    <t>Get all blog by  limit latest</t>
+  </si>
+  <si>
+    <t>get Blog by category</t>
   </si>
 </sst>
 </file>
@@ -484,7 +502,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -565,6 +583,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -663,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -738,6 +774,35 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -774,16 +839,9 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -823,7 +881,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Add to Favorites"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1159,7 +1217,7 @@
   <dimension ref="B1:C25"/>
   <sheetViews>
     <sheetView showGridLines="0" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,10 +1237,10 @@
   <sheetData>
     <row r="1" spans="2:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:3" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="33"/>
+      <c r="C2" s="44"/>
     </row>
     <row r="3" spans="2:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="13" t="s">
@@ -1377,7 +1435,7 @@
   <dimension ref="B3:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1403,7 +1461,7 @@
       <c r="D4" s="1"/>
     </row>
     <row r="5" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="48" t="s">
         <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -1412,22 +1470,22 @@
       <c r="D5" s="1"/>
     </row>
     <row r="6" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="38"/>
+      <c r="B6" s="49"/>
       <c r="C6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D6" s="1"/>
     </row>
     <row r="7" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="38"/>
+      <c r="B7" s="49"/>
       <c r="C7" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="1"/>
     </row>
     <row r="8" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="38"/>
-      <c r="C8" s="34" t="s">
+      <c r="B8" s="49"/>
+      <c r="C8" s="45" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="3" t="s">
@@ -1435,55 +1493,55 @@
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="38"/>
-      <c r="C9" s="35"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="46"/>
       <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="38"/>
-      <c r="C10" s="35"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="46"/>
       <c r="D10" s="3" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="38"/>
-      <c r="C11" s="35"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="46"/>
       <c r="D11" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="38"/>
-      <c r="C12" s="35"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="46"/>
       <c r="D12" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="38"/>
-      <c r="C13" s="35"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="46"/>
       <c r="D13" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="38"/>
-      <c r="C14" s="35"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="46"/>
       <c r="D14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="38"/>
-      <c r="C15" s="35"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="46"/>
       <c r="D15" s="6"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
-      <c r="C16" s="36"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="47"/>
       <c r="D16" s="6" t="s">
         <v>57</v>
       </c>
@@ -1527,7 +1585,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="50" t="s">
         <v>45</v>
       </c>
       <c r="D2" s="5" t="s">
@@ -1535,31 +1593,31 @@
       </c>
     </row>
     <row r="3" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C3" s="39"/>
+      <c r="C3" s="50"/>
       <c r="D3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="39"/>
+      <c r="C4" s="50"/>
       <c r="D4" s="5" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="39"/>
+      <c r="C5" s="50"/>
       <c r="D5" s="5" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="39"/>
+      <c r="C6" s="50"/>
       <c r="D6" s="5" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="39"/>
+      <c r="C7" s="50"/>
       <c r="D7" s="5" t="s">
         <v>43</v>
       </c>
@@ -1574,7 +1632,7 @@
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C10" s="39" t="s">
+      <c r="C10" s="50" t="s">
         <v>30</v>
       </c>
       <c r="D10" s="5" t="s">
@@ -1582,25 +1640,25 @@
       </c>
     </row>
     <row r="11" spans="3:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="39"/>
+      <c r="C11" s="50"/>
       <c r="D11" s="5" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C12" s="39"/>
+      <c r="C12" s="50"/>
       <c r="D12" s="5" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="13" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C13" s="39"/>
+      <c r="C13" s="50"/>
       <c r="D13" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="16" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C16" s="40" t="s">
+      <c r="C16" s="51" t="s">
         <v>33</v>
       </c>
       <c r="D16" s="5" t="s">
@@ -1608,49 +1666,49 @@
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="41"/>
+      <c r="C17" s="52"/>
       <c r="D17" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C18" s="41"/>
+      <c r="C18" s="52"/>
       <c r="D18" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C19" s="41"/>
+      <c r="C19" s="52"/>
       <c r="D19" s="5" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C20" s="41"/>
+      <c r="C20" s="52"/>
       <c r="D20" s="5" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C21" s="41"/>
+      <c r="C21" s="52"/>
       <c r="D21" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C22" s="41"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="5" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C23" s="41"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="5" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C24" s="41"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="5" t="s">
         <v>111</v>
       </c>
@@ -1675,10 +1733,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G37"/>
+  <dimension ref="C3:G41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39:G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +1764,7 @@
       </c>
     </row>
     <row r="4" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C4" s="43" t="s">
+      <c r="C4" s="54" t="s">
         <v>50</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -1723,7 +1781,7 @@
       </c>
     </row>
     <row r="5" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C5" s="43"/>
+      <c r="C5" s="54"/>
       <c r="D5" s="1" t="s">
         <v>51</v>
       </c>
@@ -1738,7 +1796,7 @@
       </c>
     </row>
     <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C6" s="43"/>
+      <c r="C6" s="54"/>
       <c r="D6" s="1" t="s">
         <v>53</v>
       </c>
@@ -1753,7 +1811,7 @@
       </c>
     </row>
     <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="43"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="1" t="s">
         <v>54</v>
       </c>
@@ -1768,7 +1826,7 @@
       </c>
     </row>
     <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="43"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="1" t="s">
         <v>55</v>
       </c>
@@ -1783,7 +1841,7 @@
       </c>
     </row>
     <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="43"/>
+      <c r="C9" s="54"/>
       <c r="D9" s="1" t="s">
         <v>56</v>
       </c>
@@ -1798,7 +1856,7 @@
       </c>
     </row>
     <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="43"/>
+      <c r="C10" s="54"/>
       <c r="D10" s="1" t="s">
         <v>57</v>
       </c>
@@ -1813,7 +1871,7 @@
       </c>
     </row>
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="43"/>
+      <c r="C11" s="54"/>
       <c r="D11" s="1" t="s">
         <v>121</v>
       </c>
@@ -1828,7 +1886,7 @@
       </c>
     </row>
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="43"/>
+      <c r="C12" s="54"/>
       <c r="D12" s="1" t="s">
         <v>122</v>
       </c>
@@ -1843,7 +1901,7 @@
       </c>
     </row>
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="43"/>
+      <c r="C13" s="54"/>
       <c r="D13" s="1" t="s">
         <v>123</v>
       </c>
@@ -1858,7 +1916,7 @@
       </c>
     </row>
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="43"/>
+      <c r="C14" s="54"/>
       <c r="D14" s="1" t="s">
         <v>118</v>
       </c>
@@ -1873,7 +1931,7 @@
       </c>
     </row>
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="43"/>
+      <c r="C15" s="54"/>
       <c r="D15" s="1" t="s">
         <v>119</v>
       </c>
@@ -1888,7 +1946,7 @@
       </c>
     </row>
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="43"/>
+      <c r="C16" s="54"/>
       <c r="D16" s="1" t="s">
         <v>120</v>
       </c>
@@ -1910,13 +1968,13 @@
       <c r="G17" s="21"/>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="42" t="s">
+      <c r="C18" s="53" t="s">
         <v>58</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="32" t="s">
         <v>115</v>
       </c>
       <c r="F18" s="24">
@@ -1927,7 +1985,7 @@
       </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C19" s="42"/>
+      <c r="C19" s="53"/>
       <c r="D19" s="1" t="s">
         <v>59</v>
       </c>
@@ -1942,7 +2000,7 @@
       </c>
     </row>
     <row r="20" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C20" s="42"/>
+      <c r="C20" s="53"/>
       <c r="D20" s="1" t="s">
         <v>61</v>
       </c>
@@ -1957,7 +2015,7 @@
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="42"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="1" t="s">
         <v>60</v>
       </c>
@@ -1972,7 +2030,7 @@
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="42"/>
+      <c r="C22" s="53"/>
       <c r="D22" s="1" t="s">
         <v>62</v>
       </c>
@@ -1987,184 +2045,256 @@
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="42"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="42"/>
+      <c r="C24" s="53"/>
       <c r="D24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F24" s="46">
+      <c r="E24" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F24" s="34">
         <v>1</v>
       </c>
-      <c r="G24" s="47">
+      <c r="G24" s="35">
         <v>45769</v>
       </c>
     </row>
     <row r="25" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C25" s="42"/>
+      <c r="C25" s="53"/>
       <c r="D25" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F25" s="46">
+      <c r="E25" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F25" s="34">
         <v>1</v>
       </c>
-      <c r="G25" s="47">
+      <c r="G25" s="35">
         <v>45769</v>
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="42"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F26" s="46">
+      <c r="E26" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F26" s="34">
         <v>1</v>
       </c>
-      <c r="G26" s="47">
+      <c r="G26" s="35">
         <v>45769</v>
       </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="42"/>
+      <c r="C27" s="53"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="42"/>
+      <c r="C28" s="53"/>
       <c r="D28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E28" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F28" s="46">
+      <c r="E28" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="34">
         <v>1</v>
       </c>
-      <c r="G28" s="47">
+      <c r="G28" s="35">
         <v>45769</v>
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="42"/>
+      <c r="C29" s="53"/>
       <c r="D29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F29" s="46">
+      <c r="E29" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F29" s="34">
         <v>1</v>
       </c>
-      <c r="G29" s="47">
+      <c r="G29" s="35">
         <v>45769</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="42"/>
+      <c r="C30" s="53"/>
       <c r="D30" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E30" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F30" s="46">
+      <c r="E30" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F30" s="34">
         <v>1</v>
       </c>
-      <c r="G30" s="47">
+      <c r="G30" s="35">
         <v>45769</v>
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="42"/>
+      <c r="C31" s="53"/>
       <c r="D31" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F31" s="46">
+      <c r="E31" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F31" s="34">
         <v>1</v>
       </c>
-      <c r="G31" s="47">
+      <c r="G31" s="35">
         <v>45769</v>
       </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="42"/>
+      <c r="C32" s="53"/>
       <c r="D32" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E32" s="45" t="s">
-        <v>115</v>
-      </c>
-      <c r="F32" s="46">
+      <c r="E32" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="F32" s="34">
         <v>1</v>
       </c>
-      <c r="G32" s="47">
+      <c r="G32" s="35">
         <v>45769</v>
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="42"/>
+      <c r="C33" s="53"/>
       <c r="D33" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E33" s="1"/>
+      <c r="E33" s="39" t="s">
+        <v>129</v>
+      </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="21"/>
+    <row r="34" spans="3:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C34" s="36"/>
       <c r="D34" s="21"/>
       <c r="E34" s="21"/>
       <c r="F34" s="21"/>
       <c r="G34" s="21"/>
     </row>
-    <row r="35" spans="3:7" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C35" s="21"/>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="21"/>
-    </row>
-    <row r="36" spans="3:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="C36" s="21"/>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="21"/>
-    </row>
-    <row r="37" spans="3:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C37" s="8" t="s">
+    <row r="35" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C35" s="55" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="E35" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="F35" s="41">
+        <v>4</v>
+      </c>
+      <c r="G35" s="42">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C36" s="55"/>
+      <c r="D36" s="38" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="F36" s="41">
+        <v>4</v>
+      </c>
+      <c r="G36" s="42">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C37" s="55"/>
+      <c r="D37" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="E37" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="F37" s="41">
+        <v>1</v>
+      </c>
+      <c r="G37" s="42">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C38" s="55"/>
+      <c r="D38" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="F38" s="41">
+        <v>1</v>
+      </c>
+      <c r="G38" s="42">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="55"/>
+      <c r="D39" s="38" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="40" t="s">
+        <v>115</v>
+      </c>
+      <c r="F39" s="41">
+        <v>1</v>
+      </c>
+      <c r="G39" s="42">
+        <v>45770</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+    </row>
+    <row r="41" spans="3:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C41" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D41" s="8">
         <v>12</v>
       </c>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="C18:C33"/>
     <mergeCell ref="C4:C16"/>
+    <mergeCell ref="C35:C39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
master class/subject/price api and superadmin validation in api
</commit_message>
<xml_diff>
--- a/edus project timeline and cost 21-april-2025.xlsx
+++ b/edus project timeline and cost 21-april-2025.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="135">
   <si>
     <t>admin_permissions</t>
   </si>
@@ -381,9 +381,6 @@
     <t>Done</t>
   </si>
   <si>
-    <t>Add Create super_amdin and admin and users</t>
-  </si>
-  <si>
     <t>Total APIs</t>
   </si>
   <si>
@@ -427,6 +424,18 @@
   </si>
   <si>
     <t>get Blog by category</t>
+  </si>
+  <si>
+    <t>Master</t>
+  </si>
+  <si>
+    <t>Master - Class</t>
+  </si>
+  <si>
+    <t>Master - Subject</t>
+  </si>
+  <si>
+    <t>Master - Price</t>
   </si>
 </sst>
 </file>
@@ -699,7 +708,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -840,6 +849,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -881,7 +899,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Add to Favorites"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1733,10 +1751,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:G41"/>
+  <dimension ref="C1:G45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39:G39"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41:C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1748,7 +1766,9 @@
     <col min="7" max="7" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="3:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="19"/>
       <c r="D3" s="20" t="s">
         <v>52</v>
@@ -1757,7 +1777,7 @@
         <v>113</v>
       </c>
       <c r="F3" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>114</v>
@@ -1767,9 +1787,7 @@
       <c r="C4" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>116</v>
-      </c>
+      <c r="D4" s="1"/>
       <c r="E4" s="28" t="s">
         <v>115</v>
       </c>
@@ -1873,7 +1891,7 @@
     <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C11" s="54"/>
       <c r="D11" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E11" s="30" t="s">
         <v>115</v>
@@ -1888,7 +1906,7 @@
     <row r="12" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C12" s="54"/>
       <c r="D12" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E12" s="30" t="s">
         <v>115</v>
@@ -1903,7 +1921,7 @@
     <row r="13" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C13" s="54"/>
       <c r="D13" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E13" s="30" t="s">
         <v>115</v>
@@ -1918,7 +1936,7 @@
     <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C14" s="54"/>
       <c r="D14" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>115</v>
@@ -1933,7 +1951,7 @@
     <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C15" s="54"/>
       <c r="D15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E15" s="30" t="s">
         <v>115</v>
@@ -1948,7 +1966,7 @@
     <row r="16" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C16" s="54"/>
       <c r="D16" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E16" s="30" t="s">
         <v>115</v>
@@ -2136,7 +2154,7 @@
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="53"/>
       <c r="D30" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E30" s="33" t="s">
         <v>115</v>
@@ -2166,7 +2184,7 @@
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C32" s="53"/>
       <c r="D32" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E32" s="33" t="s">
         <v>115</v>
@@ -2184,7 +2202,7 @@
         <v>69</v>
       </c>
       <c r="E33" s="39" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
@@ -2201,7 +2219,7 @@
         <v>112</v>
       </c>
       <c r="D35" s="37" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E35" s="40" t="s">
         <v>115</v>
@@ -2216,7 +2234,7 @@
     <row r="36" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C36" s="55"/>
       <c r="D36" s="38" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E36" s="40" t="s">
         <v>115</v>
@@ -2231,7 +2249,7 @@
     <row r="37" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="55"/>
       <c r="D37" s="38" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E37" s="40" t="s">
         <v>115</v>
@@ -2246,7 +2264,7 @@
     <row r="38" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="55"/>
       <c r="D38" s="38" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E38" s="40" t="s">
         <v>115</v>
@@ -2261,7 +2279,7 @@
     <row r="39" spans="3:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="55"/>
       <c r="D39" s="38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E39" s="40" t="s">
         <v>115</v>
@@ -2273,28 +2291,70 @@
         <v>45770</v>
       </c>
     </row>
-    <row r="40" spans="3:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C40" s="21"/>
-      <c r="E40" s="21"/>
-      <c r="F40" s="21"/>
-      <c r="G40" s="21"/>
-    </row>
-    <row r="41" spans="3:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C41" s="8" t="s">
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F41" s="25">
+        <v>4</v>
+      </c>
+      <c r="G41" s="42">
+        <v>45771</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="57"/>
+      <c r="D42" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E42" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="25">
+        <v>4</v>
+      </c>
+      <c r="G42" s="42">
+        <v>45771</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="58"/>
+      <c r="D43" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="F43" s="25">
+        <v>4</v>
+      </c>
+      <c r="G43" s="42">
+        <v>45771</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C45" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D41" s="8">
+      <c r="D45" s="8">
         <v>12</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="C18:C33"/>
     <mergeCell ref="C4:C16"/>
     <mergeCell ref="C35:C39"/>
+    <mergeCell ref="C41:C43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>